<commit_message>
Updated template and schema
</commit_message>
<xml_diff>
--- a/inst/extdata/COP25_Data_Pack_Template.xlsx
+++ b/inst/extdata/COP25_Data_Pack_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d-christian.domaas\Documents\GitHub\datapackr\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DAD229D2-55C1-4EDB-A22F-C60AF4BE40A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3302EE4-5E5E-484D-B9E0-22F0EF9A7E87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-3405" windowWidth="38640" windowHeight="21240" firstSheet="1" activeTab="3" xr2:uid="{35D0834B-83BC-CC4F-BCCA-B5B2ECED3698}"/>
+    <workbookView xWindow="-38520" yWindow="-3405" windowWidth="38640" windowHeight="21240" firstSheet="1" activeTab="14" xr2:uid="{35D0834B-83BC-CC4F-BCCA-B5B2ECED3698}"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="1" r:id="rId1"/>
@@ -7824,7 +7824,7 @@
       <pane xSplit="5" ySplit="14" topLeftCell="F15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B14" sqref="B14"/>
+      <selection pane="bottomRight" activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -8524,11 +8524,11 @@
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:T15"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="5" ySplit="14" topLeftCell="F15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B14" sqref="B14"/>
+      <selection pane="bottomRight" activeCell="T15" sqref="T15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -9251,11 +9251,11 @@
         <v/>
       </c>
       <c r="S15" s="33" t="str">
-        <f>$N15</f>
+        <f>IF(SUM($N15)=0,"",$N15)</f>
         <v/>
       </c>
       <c r="T15" s="33" t="str">
-        <f>IF(SUM($O15)=0,"",ROUND($O15*SUM(#REF!),0))</f>
+        <f>IF(SUM($O15)=0,"",$O15)</f>
         <v/>
       </c>
     </row>
@@ -9277,7 +9277,7 @@
       <formula>AND(ISNUMBER(Q2),Q2&gt;1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q1:T1 R2:T14 Q15:T1048576 F1:P1048576">
+  <conditionalFormatting sqref="Q1:T1 R2:T14 F1:P1048576 Q15:T1048576">
     <cfRule type="expression" dxfId="1" priority="14">
       <formula>AND(ISNUMBER(F1),F1&lt;0)</formula>
     </cfRule>
@@ -23398,7 +23398,7 @@
   <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:BF3876"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="5" ySplit="14" topLeftCell="F15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>

</xml_diff>